<commit_message>
Miss match bug fixed
</commit_message>
<xml_diff>
--- a/data/GroundTruth/LandCover.xlsx
+++ b/data/GroundTruth/LandCover.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YunzZhu\Box\2022_Spring\STA208\FinalProject\STA_208_Final_RS_Classification\data\GroundTruth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4680F788-590C-4B89-A3D1-B147F8ED29A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CAAE88-6DE0-4769-9778-CCE49CB574CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="2370" windowWidth="18645" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LandCover" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="103">
   <si>
     <t>groundType</t>
   </si>
@@ -668,7 +668,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -845,6 +845,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -890,7 +945,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -901,6 +956,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1256,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:H22"/>
+      <selection activeCell="F2" sqref="F2:F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,7 +1335,7 @@
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1288,7 +1349,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1302,10 +1363,15 @@
         <v>86</v>
       </c>
       <c r="E2">
+        <f t="shared" ref="E2:F34" si="0">VLOOKUP(D2,$G$3:$H$22,2,FALSE)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>VLOOKUP(D2,$I$3:$J$22,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1319,17 +1385,27 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f>VLOOKUP(D3,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="1">VLOOKUP(D3,$I$3:$J$22,2,FALSE)</f>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1343,17 +1419,27 @@
         <v>22</v>
       </c>
       <c r="E4">
-        <f>VLOOKUP(D4,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1367,17 +1453,27 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <f>VLOOKUP(D5,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1391,17 +1487,27 @@
         <v>88</v>
       </c>
       <c r="E6">
-        <f>VLOOKUP(D6,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="15">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1415,17 +1521,27 @@
         <v>99</v>
       </c>
       <c r="E7">
-        <f>VLOOKUP(D7,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1439,17 +1555,27 @@
         <v>94</v>
       </c>
       <c r="E8">
-        <f>VLOOKUP(D8,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="14">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -1463,17 +1589,27 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <f>VLOOKUP(D9,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="14">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>13</v>
       </c>
@@ -1487,17 +1623,27 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <f>VLOOKUP(D10,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="15">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
@@ -1511,17 +1657,27 @@
         <v>18</v>
       </c>
       <c r="E11">
-        <f>VLOOKUP(D11,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="14">
+        <v>9</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>21</v>
       </c>
@@ -1535,17 +1691,27 @@
         <v>88</v>
       </c>
       <c r="E12">
-        <f>VLOOKUP(D12,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="14">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>22</v>
       </c>
@@ -1559,17 +1725,27 @@
         <v>88</v>
       </c>
       <c r="E13">
-        <f>VLOOKUP(D13,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>23</v>
       </c>
@@ -1583,17 +1759,27 @@
         <v>88</v>
       </c>
       <c r="E14">
-        <f>VLOOKUP(D14,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>24</v>
       </c>
@@ -1607,17 +1793,27 @@
         <v>88</v>
       </c>
       <c r="E15">
-        <f>VLOOKUP(D15,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="14">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>27</v>
       </c>
@@ -1631,17 +1827,27 @@
         <v>88</v>
       </c>
       <c r="E16">
-        <f>VLOOKUP(D16,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="14">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>28</v>
       </c>
@@ -1655,17 +1861,27 @@
         <v>88</v>
       </c>
       <c r="E17">
-        <f>VLOOKUP(D17,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="14">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>29</v>
       </c>
@@ -1679,17 +1895,27 @@
         <v>88</v>
       </c>
       <c r="E18">
-        <f>VLOOKUP(D18,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="14">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>31</v>
       </c>
@@ -1703,17 +1929,27 @@
         <v>94</v>
       </c>
       <c r="E19">
-        <f>VLOOKUP(D19,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="14">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>33</v>
       </c>
@@ -1727,17 +1963,27 @@
         <v>94</v>
       </c>
       <c r="E20">
-        <f>VLOOKUP(D20,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="14">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>36</v>
       </c>
@@ -1751,17 +1997,27 @@
         <v>18</v>
       </c>
       <c r="E21">
-        <f>VLOOKUP(D21,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="14">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>37</v>
       </c>
@@ -1775,17 +2031,27 @@
         <v>95</v>
       </c>
       <c r="E22">
-        <f>VLOOKUP(D22,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="15">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>39</v>
       </c>
@@ -1799,11 +2065,15 @@
         <v>88</v>
       </c>
       <c r="E23">
-        <f>VLOOKUP(D23,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>42</v>
       </c>
@@ -1817,11 +2087,15 @@
         <v>98</v>
       </c>
       <c r="E24">
-        <f>VLOOKUP(D24,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>43</v>
       </c>
@@ -1835,11 +2109,15 @@
         <v>98</v>
       </c>
       <c r="E25">
-        <f>VLOOKUP(D25,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>44</v>
       </c>
@@ -1853,11 +2131,15 @@
         <v>22</v>
       </c>
       <c r="E26">
-        <f>VLOOKUP(D26,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>46</v>
       </c>
@@ -1871,11 +2153,15 @@
         <v>98</v>
       </c>
       <c r="E27">
-        <f>VLOOKUP(D27,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>47</v>
       </c>
@@ -1889,11 +2175,15 @@
         <v>22</v>
       </c>
       <c r="E28">
-        <f>VLOOKUP(D28,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>48</v>
       </c>
@@ -1907,11 +2197,15 @@
         <v>99</v>
       </c>
       <c r="E29">
-        <f>VLOOKUP(D29,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>49</v>
       </c>
@@ -1925,11 +2219,15 @@
         <v>99</v>
       </c>
       <c r="E30">
-        <f>VLOOKUP(D30,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>50</v>
       </c>
@@ -1943,11 +2241,15 @@
         <v>99</v>
       </c>
       <c r="E31">
-        <f>VLOOKUP(D31,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>51</v>
       </c>
@@ -1961,11 +2263,15 @@
         <v>88</v>
       </c>
       <c r="E32">
-        <f>VLOOKUP(D32,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>53</v>
       </c>
@@ -1979,11 +2285,15 @@
         <v>99</v>
       </c>
       <c r="E33">
-        <f>VLOOKUP(D33,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>54</v>
       </c>
@@ -1997,11 +2307,15 @@
         <v>99</v>
       </c>
       <c r="E34">
-        <f>VLOOKUP(D34,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>57</v>
       </c>
@@ -2015,11 +2329,15 @@
         <v>18</v>
       </c>
       <c r="E35">
-        <f>VLOOKUP(D35,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" ref="E35:E66" si="2">VLOOKUP(D35,$G$3:$H$22,2,FALSE)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>58</v>
       </c>
@@ -2033,11 +2351,15 @@
         <v>94</v>
       </c>
       <c r="E36">
-        <f>VLOOKUP(D36,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>59</v>
       </c>
@@ -2051,11 +2373,15 @@
         <v>85</v>
       </c>
       <c r="E37">
-        <f>VLOOKUP(D37,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>61</v>
       </c>
@@ -2069,11 +2395,15 @@
         <v>92</v>
       </c>
       <c r="E38">
-        <f>VLOOKUP(D38,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>66</v>
       </c>
@@ -2087,11 +2417,15 @@
         <v>97</v>
       </c>
       <c r="E39">
-        <f>VLOOKUP(D39,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>67</v>
       </c>
@@ -2105,11 +2439,15 @@
         <v>97</v>
       </c>
       <c r="E40">
-        <f>VLOOKUP(D40,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>68</v>
       </c>
@@ -2123,11 +2461,15 @@
         <v>97</v>
       </c>
       <c r="E41">
-        <f>VLOOKUP(D41,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>69</v>
       </c>
@@ -2141,11 +2483,15 @@
         <v>38</v>
       </c>
       <c r="E42">
-        <f>VLOOKUP(D42,$G$3:$H$22,2,FALSE)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>70</v>
       </c>
@@ -2159,11 +2505,15 @@
         <v>97</v>
       </c>
       <c r="E43">
-        <f>VLOOKUP(D43,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>71</v>
       </c>
@@ -2177,11 +2527,15 @@
         <v>97</v>
       </c>
       <c r="E44">
-        <f>VLOOKUP(D44,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>72</v>
       </c>
@@ -2195,11 +2549,15 @@
         <v>97</v>
       </c>
       <c r="E45">
-        <f>VLOOKUP(D45,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>74</v>
       </c>
@@ -2213,11 +2571,15 @@
         <v>96</v>
       </c>
       <c r="E46">
-        <f>VLOOKUP(D46,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>75</v>
       </c>
@@ -2231,11 +2593,15 @@
         <v>96</v>
       </c>
       <c r="E47">
-        <f>VLOOKUP(D47,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>76</v>
       </c>
@@ -2249,11 +2615,15 @@
         <v>96</v>
       </c>
       <c r="E48">
-        <f>VLOOKUP(D48,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>77</v>
       </c>
@@ -2267,11 +2637,15 @@
         <v>97</v>
       </c>
       <c r="E49">
-        <f>VLOOKUP(D49,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>92</v>
       </c>
@@ -2285,11 +2659,15 @@
         <v>86</v>
       </c>
       <c r="E50">
-        <f>VLOOKUP(D50,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>111</v>
       </c>
@@ -2303,11 +2681,15 @@
         <v>86</v>
       </c>
       <c r="E51">
-        <f>VLOOKUP(D51,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>112</v>
       </c>
@@ -2321,11 +2703,15 @@
         <v>86</v>
       </c>
       <c r="E52">
-        <f>VLOOKUP(D52,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>121</v>
       </c>
@@ -2339,11 +2725,15 @@
         <v>90</v>
       </c>
       <c r="E53">
-        <f>VLOOKUP(D53,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>122</v>
       </c>
@@ -2357,11 +2747,15 @@
         <v>90</v>
       </c>
       <c r="E54">
-        <f>VLOOKUP(D54,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>123</v>
       </c>
@@ -2375,11 +2769,15 @@
         <v>90</v>
       </c>
       <c r="E55">
-        <f>VLOOKUP(D55,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>124</v>
       </c>
@@ -2393,11 +2791,15 @@
         <v>90</v>
       </c>
       <c r="E56">
-        <f>VLOOKUP(D56,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>131</v>
       </c>
@@ -2411,11 +2813,15 @@
         <v>53</v>
       </c>
       <c r="E57">
-        <f>VLOOKUP(D57,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>141</v>
       </c>
@@ -2429,11 +2835,15 @@
         <v>87</v>
       </c>
       <c r="E58">
-        <f>VLOOKUP(D58,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>142</v>
       </c>
@@ -2447,11 +2857,15 @@
         <v>87</v>
       </c>
       <c r="E59">
-        <f>VLOOKUP(D59,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>143</v>
       </c>
@@ -2465,11 +2879,15 @@
         <v>87</v>
       </c>
       <c r="E60">
-        <f>VLOOKUP(D60,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>152</v>
       </c>
@@ -2483,11 +2901,15 @@
         <v>57</v>
       </c>
       <c r="E61">
-        <f>VLOOKUP(D61,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>176</v>
       </c>
@@ -2501,11 +2923,15 @@
         <v>85</v>
       </c>
       <c r="E62">
-        <f>VLOOKUP(D62,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>190</v>
       </c>
@@ -2519,11 +2945,15 @@
         <v>91</v>
       </c>
       <c r="E63">
-        <f>VLOOKUP(D63,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>195</v>
       </c>
@@ -2537,11 +2967,15 @@
         <v>91</v>
       </c>
       <c r="E64">
-        <f>VLOOKUP(D64,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>204</v>
       </c>
@@ -2555,11 +2989,15 @@
         <v>96</v>
       </c>
       <c r="E65">
-        <f>VLOOKUP(D65,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>205</v>
       </c>
@@ -2573,11 +3011,15 @@
         <v>88</v>
       </c>
       <c r="E66">
-        <f>VLOOKUP(D66,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>206</v>
       </c>
@@ -2591,11 +3033,15 @@
         <v>99</v>
       </c>
       <c r="E67">
-        <f>VLOOKUP(D67,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" ref="E67:E98" si="3">VLOOKUP(D67,$G$3:$H$22,2,FALSE)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" ref="F67:F89" si="4">VLOOKUP(D67,$I$3:$J$22,2,FALSE)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>208</v>
       </c>
@@ -2609,11 +3055,15 @@
         <v>99</v>
       </c>
       <c r="E68">
-        <f>VLOOKUP(D68,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>209</v>
       </c>
@@ -2627,11 +3077,15 @@
         <v>99</v>
       </c>
       <c r="E69">
-        <f>VLOOKUP(D69,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>211</v>
       </c>
@@ -2645,11 +3099,15 @@
         <v>96</v>
       </c>
       <c r="E70">
-        <f>VLOOKUP(D70,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>212</v>
       </c>
@@ -2663,11 +3121,15 @@
         <v>97</v>
       </c>
       <c r="E71">
-        <f>VLOOKUP(D71,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>213</v>
       </c>
@@ -2681,11 +3143,15 @@
         <v>99</v>
       </c>
       <c r="E72">
-        <f>VLOOKUP(D72,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>214</v>
       </c>
@@ -2699,11 +3165,15 @@
         <v>99</v>
       </c>
       <c r="E73">
-        <f>VLOOKUP(D73,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>216</v>
       </c>
@@ -2717,11 +3187,15 @@
         <v>99</v>
       </c>
       <c r="E74">
-        <f>VLOOKUP(D74,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>217</v>
       </c>
@@ -2735,11 +3209,15 @@
         <v>97</v>
       </c>
       <c r="E75">
-        <f>VLOOKUP(D75,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>218</v>
       </c>
@@ -2753,11 +3231,15 @@
         <v>97</v>
       </c>
       <c r="E76">
-        <f>VLOOKUP(D76,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>219</v>
       </c>
@@ -2771,11 +3253,15 @@
         <v>99</v>
       </c>
       <c r="E77">
-        <f>VLOOKUP(D77,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>220</v>
       </c>
@@ -2789,11 +3275,15 @@
         <v>97</v>
       </c>
       <c r="E78">
-        <f>VLOOKUP(D78,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>221</v>
       </c>
@@ -2807,11 +3297,15 @@
         <v>22</v>
       </c>
       <c r="E79">
-        <f>VLOOKUP(D79,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>222</v>
       </c>
@@ -2825,11 +3319,15 @@
         <v>99</v>
       </c>
       <c r="E80">
-        <f>VLOOKUP(D80,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>224</v>
       </c>
@@ -2843,11 +3341,15 @@
         <v>94</v>
       </c>
       <c r="E81">
-        <f>VLOOKUP(D81,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>225</v>
       </c>
@@ -2861,11 +3363,15 @@
         <v>2</v>
       </c>
       <c r="E82">
-        <f>VLOOKUP(D82,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>226</v>
       </c>
@@ -2879,11 +3385,15 @@
         <v>2</v>
       </c>
       <c r="E83">
-        <f>VLOOKUP(D83,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>227</v>
       </c>
@@ -2897,11 +3407,15 @@
         <v>99</v>
       </c>
       <c r="E84">
-        <f>VLOOKUP(D84,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>228</v>
       </c>
@@ -2915,11 +3429,15 @@
         <v>2</v>
       </c>
       <c r="E85">
-        <f>VLOOKUP(D85,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>229</v>
       </c>
@@ -2933,11 +3451,15 @@
         <v>99</v>
       </c>
       <c r="E86">
-        <f>VLOOKUP(D86,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>236</v>
       </c>
@@ -2951,11 +3473,15 @@
         <v>88</v>
       </c>
       <c r="E87">
-        <f>VLOOKUP(D87,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>242</v>
       </c>
@@ -2969,11 +3495,15 @@
         <v>99</v>
       </c>
       <c r="E88">
-        <f>VLOOKUP(D88,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>243</v>
       </c>
@@ -2987,17 +3517,21 @@
         <v>99</v>
       </c>
       <c r="E89">
-        <f>VLOOKUP(D89,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B90" s="1">
         <f>SUM(B2:B89)</f>
         <v>15709188</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Go through before presentation
</commit_message>
<xml_diff>
--- a/data/GroundTruth/LandCover.xlsx
+++ b/data/GroundTruth/LandCover.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YunzZhu\Box\2022_Spring\STA208\FinalProject\STA_208_Final_RS_Classification\data\GroundTruth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CAAE88-6DE0-4769-9778-CCE49CB574CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5466FFD8-2582-4D50-AD54-F48D80C8DC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LandCover" sheetId="1" r:id="rId1"/>
@@ -1320,7 +1320,7 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F89"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1363,7 @@
         <v>86</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:F34" si="0">VLOOKUP(D2,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" ref="E2:E34" si="0">VLOOKUP(D2,$G$3:$H$22,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F2">
@@ -3033,7 +3033,7 @@
         <v>99</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E98" si="3">VLOOKUP(D67,$G$3:$H$22,2,FALSE)</f>
+        <f t="shared" ref="E67:E89" si="3">VLOOKUP(D67,$G$3:$H$22,2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F67">

</xml_diff>